<commit_message>
snake_case & foreach compiler.translator
</commit_message>
<xml_diff>
--- a/examples/colors.xlsx
+++ b/examples/colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muzud\OneDrive\ドキュメント\GitHub\trellis\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D99D90A-D390-4B8A-AF51-BA565B7970D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82502EA4-D9C9-4F55-BD8E-72619A5BE819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3350" yWindow="280" windowWidth="14080" windowHeight="15880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="490" windowWidth="30190" windowHeight="18230" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,15 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="96">
-  <si>
-    <t>blue</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>green</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>#5B9BD5</t>
     <phoneticPr fontId="1"/>
@@ -90,14 +82,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>standard</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>gray</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#3A3838</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -159,90 +143,6 @@
   </si>
   <si>
     <t>#7030A0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_pale</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_light</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_soft</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_strong</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_deep</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_white</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_black</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_red_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_blue_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_blue</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_brown</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_gray</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_yellow</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_green</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_red</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_orange</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_yellow_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_dodger_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_naviy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>xl_violet</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -334,10 +234,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>xl_theme</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#000000</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -419,6 +315,94 @@
   </si>
   <si>
     <t>#375623</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlWhite</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlBlack</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlRedGray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlBlueGray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlBlue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlRed</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlGray</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlYellow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlNaviy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlGreen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlTheme</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlPale</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlLight</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlSoft</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlStrong</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlDeep</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlBrown</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlStandard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlOrange</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlYellowGreen</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlDodgerBlue</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>xlViolet</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1809,952 +1793,939 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:AG32"/>
+  <dimension ref="C2:AJ32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AH29" sqref="AH29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.4140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="16384" width="2.4140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:33" ht="15" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="4:36" ht="15" customHeight="1">
+      <c r="D2" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="4:36" ht="15" customHeight="1">
+      <c r="G4" s="551" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="4:36" ht="15" customHeight="1">
+      <c r="G5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH5" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="4:36" ht="15" customHeight="1" thickBot="1">
+      <c r="P6" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:33" ht="15" customHeight="1">
-      <c r="D4" s="551" t="s">
-        <v>71</v>
-      </c>
+    <row r="7" spans="4:36" ht="15" customHeight="1">
+      <c r="D7" s="551" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="125"/>
+      <c r="H7" s="126"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="345"/>
+      <c r="N7" s="346"/>
+      <c r="O7" s="347"/>
+      <c r="P7" s="354"/>
+      <c r="Q7" s="355"/>
+      <c r="R7" s="356"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="30"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="77"/>
+      <c r="W7" s="78"/>
+      <c r="X7" s="79"/>
+      <c r="Y7" s="381"/>
+      <c r="Z7" s="382"/>
+      <c r="AA7" s="383"/>
+      <c r="AB7" s="164"/>
+      <c r="AC7" s="165"/>
+      <c r="AD7" s="166"/>
+      <c r="AE7" s="254"/>
+      <c r="AF7" s="255"/>
+      <c r="AG7" s="256"/>
+      <c r="AH7" s="257"/>
+      <c r="AI7" s="258"/>
+      <c r="AJ7" s="259"/>
     </row>
-    <row r="5" spans="1:33" ht="15" customHeight="1">
-      <c r="D5" s="1" t="s">
+    <row r="8" spans="4:36" ht="15" customHeight="1">
+      <c r="D8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="138" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="139"/>
+      <c r="I8" s="140"/>
+      <c r="J8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="200"/>
+      <c r="L8" s="201"/>
+      <c r="M8" s="348" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="349"/>
+      <c r="O8" s="350"/>
+      <c r="P8" s="438" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q8" s="439"/>
+      <c r="R8" s="440"/>
+      <c r="S8" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" s="42"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="89" t="s">
+        <v>2</v>
+      </c>
+      <c r="W8" s="90"/>
+      <c r="X8" s="91"/>
+      <c r="Y8" s="384" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z8" s="385"/>
+      <c r="AA8" s="386"/>
+      <c r="AB8" s="176" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC8" s="177"/>
+      <c r="AD8" s="178"/>
+      <c r="AE8" s="113" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="114"/>
+      <c r="AG8" s="115"/>
+      <c r="AH8" s="65" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI8" s="66"/>
+      <c r="AJ8" s="67"/>
+    </row>
+    <row r="9" spans="4:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G9" s="151"/>
+      <c r="H9" s="152"/>
+      <c r="I9" s="153"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="351"/>
+      <c r="N9" s="352"/>
+      <c r="O9" s="353"/>
+      <c r="P9" s="357"/>
+      <c r="Q9" s="358"/>
+      <c r="R9" s="359"/>
+      <c r="S9" s="53"/>
+      <c r="T9" s="54"/>
+      <c r="U9" s="55"/>
+      <c r="V9" s="101"/>
+      <c r="W9" s="102"/>
+      <c r="X9" s="103"/>
+      <c r="Y9" s="387"/>
+      <c r="Z9" s="388"/>
+      <c r="AA9" s="389"/>
+      <c r="AB9" s="188"/>
+      <c r="AC9" s="189"/>
+      <c r="AD9" s="190"/>
+      <c r="AE9" s="260"/>
+      <c r="AF9" s="261"/>
+      <c r="AG9" s="262"/>
+      <c r="AH9" s="263"/>
+      <c r="AI9" s="264"/>
+      <c r="AJ9" s="265"/>
+    </row>
+    <row r="10" spans="4:36" ht="15" customHeight="1" thickBot="1"/>
+    <row r="11" spans="4:36" ht="15" customHeight="1">
+      <c r="G11" s="128"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="411"/>
+      <c r="N11" s="412"/>
+      <c r="O11" s="413"/>
+      <c r="P11" s="360"/>
+      <c r="Q11" s="361"/>
+      <c r="R11" s="362"/>
+      <c r="S11" s="32"/>
+      <c r="T11" s="33"/>
+      <c r="U11" s="34"/>
+      <c r="V11" s="80"/>
+      <c r="W11" s="81"/>
+      <c r="X11" s="82"/>
+      <c r="Y11" s="396"/>
+      <c r="Z11" s="397"/>
+      <c r="AA11" s="398"/>
+      <c r="AB11" s="167"/>
+      <c r="AC11" s="168"/>
+      <c r="AD11" s="169"/>
+      <c r="AE11" s="218"/>
+      <c r="AF11" s="219"/>
+      <c r="AG11" s="220"/>
+      <c r="AH11" s="221"/>
+      <c r="AI11" s="222"/>
+      <c r="AJ11" s="223"/>
+    </row>
+    <row r="12" spans="4:36" ht="15" customHeight="1">
+      <c r="D12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="141" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="142"/>
+      <c r="I12" s="143"/>
+      <c r="J12" s="202" t="s">
+        <v>7</v>
+      </c>
+      <c r="K12" s="203"/>
+      <c r="L12" s="204"/>
+      <c r="M12" s="414" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="415"/>
+      <c r="O12" s="416"/>
+      <c r="P12" s="363" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" s="364"/>
+      <c r="R12" s="365"/>
+      <c r="S12" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="T12" s="45"/>
+      <c r="U12" s="46"/>
+      <c r="V12" s="92" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" s="93"/>
+      <c r="X12" s="94"/>
+      <c r="Y12" s="399" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z12" s="400"/>
+      <c r="AA12" s="401"/>
+      <c r="AB12" s="179" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC12" s="180"/>
+      <c r="AD12" s="181"/>
+      <c r="AE12" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF12" s="117"/>
+      <c r="AG12" s="118"/>
+      <c r="AH12" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI12" s="69"/>
+      <c r="AJ12" s="70"/>
+    </row>
+    <row r="13" spans="4:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G13" s="154"/>
+      <c r="H13" s="155"/>
+      <c r="I13" s="156"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="20"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="417"/>
+      <c r="N13" s="418"/>
+      <c r="O13" s="419"/>
+      <c r="P13" s="366"/>
+      <c r="Q13" s="367"/>
+      <c r="R13" s="368"/>
+      <c r="S13" s="56"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="104"/>
+      <c r="W13" s="105"/>
+      <c r="X13" s="106"/>
+      <c r="Y13" s="402"/>
+      <c r="Z13" s="403"/>
+      <c r="AA13" s="404"/>
+      <c r="AB13" s="191"/>
+      <c r="AC13" s="192"/>
+      <c r="AD13" s="193"/>
+      <c r="AE13" s="224"/>
+      <c r="AF13" s="225"/>
+      <c r="AG13" s="226"/>
+      <c r="AH13" s="227"/>
+      <c r="AI13" s="228"/>
+      <c r="AJ13" s="229"/>
+    </row>
+    <row r="14" spans="4:36" ht="15" customHeight="1">
+      <c r="G14" s="131"/>
+      <c r="H14" s="132"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="420"/>
+      <c r="N14" s="421"/>
+      <c r="O14" s="422"/>
+      <c r="P14" s="369"/>
+      <c r="Q14" s="370"/>
+      <c r="R14" s="371"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="83"/>
+      <c r="W14" s="84"/>
+      <c r="X14" s="85"/>
+      <c r="Y14" s="390"/>
+      <c r="Z14" s="391"/>
+      <c r="AA14" s="392"/>
+      <c r="AB14" s="170"/>
+      <c r="AC14" s="171"/>
+      <c r="AD14" s="172"/>
+      <c r="AE14" s="230"/>
+      <c r="AF14" s="231"/>
+      <c r="AG14" s="232"/>
+      <c r="AH14" s="233"/>
+      <c r="AI14" s="234"/>
+      <c r="AJ14" s="235"/>
+    </row>
+    <row r="15" spans="4:36" ht="15" customHeight="1">
+      <c r="D15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="144" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="145"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="205" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="206"/>
+      <c r="L15" s="207"/>
+      <c r="M15" s="420" t="s">
+        <v>32</v>
+      </c>
+      <c r="N15" s="421"/>
+      <c r="O15" s="422"/>
+      <c r="P15" s="369" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q15" s="370"/>
+      <c r="R15" s="371"/>
+      <c r="S15" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="48"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="95" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="96"/>
+      <c r="X15" s="97"/>
+      <c r="Y15" s="390" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z15" s="391"/>
+      <c r="AA15" s="392"/>
+      <c r="AB15" s="182" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC15" s="183"/>
+      <c r="AD15" s="184"/>
+      <c r="AE15" s="119" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF15" s="120"/>
+      <c r="AG15" s="121"/>
+      <c r="AH15" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI15" s="72"/>
+      <c r="AJ15" s="73"/>
+    </row>
+    <row r="16" spans="4:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G16" s="157"/>
+      <c r="H16" s="158"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="423"/>
+      <c r="N16" s="424"/>
+      <c r="O16" s="425"/>
+      <c r="P16" s="372"/>
+      <c r="Q16" s="373"/>
+      <c r="R16" s="374"/>
+      <c r="S16" s="59"/>
+      <c r="T16" s="60"/>
+      <c r="U16" s="61"/>
+      <c r="V16" s="107"/>
+      <c r="W16" s="108"/>
+      <c r="X16" s="109"/>
+      <c r="Y16" s="393"/>
+      <c r="Z16" s="394"/>
+      <c r="AA16" s="395"/>
+      <c r="AB16" s="194"/>
+      <c r="AC16" s="195"/>
+      <c r="AD16" s="196"/>
+      <c r="AE16" s="236"/>
+      <c r="AF16" s="237"/>
+      <c r="AG16" s="238"/>
+      <c r="AH16" s="239"/>
+      <c r="AI16" s="240"/>
+      <c r="AJ16" s="241"/>
+    </row>
+    <row r="17" spans="3:36" ht="15" customHeight="1">
+      <c r="G17" s="134"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="426"/>
+      <c r="N17" s="427"/>
+      <c r="O17" s="428"/>
+      <c r="P17" s="375"/>
+      <c r="Q17" s="376"/>
+      <c r="R17" s="377"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="86"/>
+      <c r="W17" s="87"/>
+      <c r="X17" s="88"/>
+      <c r="Y17" s="405"/>
+      <c r="Z17" s="406"/>
+      <c r="AA17" s="407"/>
+      <c r="AB17" s="173"/>
+      <c r="AC17" s="174"/>
+      <c r="AD17" s="175"/>
+      <c r="AE17" s="242"/>
+      <c r="AF17" s="243"/>
+      <c r="AG17" s="244"/>
+      <c r="AH17" s="245"/>
+      <c r="AI17" s="246"/>
+      <c r="AJ17" s="247"/>
+    </row>
+    <row r="18" spans="3:36" ht="15" customHeight="1">
+      <c r="D18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="147" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H18" s="148"/>
+      <c r="I18" s="149"/>
+      <c r="J18" s="208" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K18" s="209"/>
+      <c r="L18" s="210"/>
+      <c r="M18" s="426" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" s="427"/>
+      <c r="O18" s="428"/>
+      <c r="P18" s="375" t="s">
         <v>42</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="Q18" s="376"/>
+      <c r="R18" s="377"/>
+      <c r="S18" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="T18" s="51"/>
+      <c r="U18" s="52"/>
+      <c r="V18" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="W18" s="99"/>
+      <c r="X18" s="100"/>
+      <c r="Y18" s="405" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z18" s="406"/>
+      <c r="AA18" s="407"/>
+      <c r="AB18" s="185" t="s">
         <v>43</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="AC18" s="186"/>
+      <c r="AD18" s="187"/>
+      <c r="AE18" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AF18" s="123"/>
+      <c r="AG18" s="124"/>
+      <c r="AH18" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI18" s="75"/>
+      <c r="AJ18" s="76"/>
+    </row>
+    <row r="19" spans="3:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G19" s="160"/>
+      <c r="H19" s="161"/>
+      <c r="I19" s="162"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="429"/>
+      <c r="N19" s="430"/>
+      <c r="O19" s="431"/>
+      <c r="P19" s="378"/>
+      <c r="Q19" s="379"/>
+      <c r="R19" s="380"/>
+      <c r="S19" s="62"/>
+      <c r="T19" s="63"/>
+      <c r="U19" s="64"/>
+      <c r="V19" s="110"/>
+      <c r="W19" s="111"/>
+      <c r="X19" s="112"/>
+      <c r="Y19" s="408"/>
+      <c r="Z19" s="409"/>
+      <c r="AA19" s="410"/>
+      <c r="AB19" s="197"/>
+      <c r="AC19" s="198"/>
+      <c r="AD19" s="199"/>
+      <c r="AE19" s="248"/>
+      <c r="AF19" s="249"/>
+      <c r="AG19" s="250"/>
+      <c r="AH19" s="251"/>
+      <c r="AI19" s="252"/>
+      <c r="AJ19" s="253"/>
+    </row>
+    <row r="20" spans="3:36" ht="15" customHeight="1">
+      <c r="G20" s="215"/>
+      <c r="H20" s="137"/>
+      <c r="I20" s="137"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="426"/>
+      <c r="N20" s="427"/>
+      <c r="O20" s="428"/>
+      <c r="P20" s="452"/>
+      <c r="Q20" s="453"/>
+      <c r="R20" s="454"/>
+      <c r="S20" s="459"/>
+      <c r="T20" s="459"/>
+      <c r="U20" s="459"/>
+      <c r="V20" s="470"/>
+      <c r="W20" s="470"/>
+      <c r="X20" s="470"/>
+      <c r="Y20" s="471"/>
+      <c r="Z20" s="472"/>
+      <c r="AA20" s="473"/>
+      <c r="AB20" s="474"/>
+      <c r="AC20" s="474"/>
+      <c r="AD20" s="474"/>
+      <c r="AE20" s="475"/>
+      <c r="AF20" s="476"/>
+      <c r="AG20" s="476"/>
+      <c r="AH20" s="477"/>
+      <c r="AI20" s="477"/>
+      <c r="AJ20" s="478"/>
+    </row>
+    <row r="21" spans="3:36" ht="15" customHeight="1">
+      <c r="D21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G21" s="216" t="s">
         <v>53</v>
       </c>
-      <c r="AE5" s="1" t="s">
-        <v>48</v>
-      </c>
+      <c r="H21" s="150"/>
+      <c r="I21" s="150"/>
+      <c r="J21" s="211" t="s">
+        <v>54</v>
+      </c>
+      <c r="K21" s="211"/>
+      <c r="L21" s="211"/>
+      <c r="M21" s="426" t="s">
+        <v>14</v>
+      </c>
+      <c r="N21" s="427"/>
+      <c r="O21" s="428"/>
+      <c r="P21" s="452" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q21" s="453"/>
+      <c r="R21" s="454"/>
+      <c r="S21" s="458" t="s">
+        <v>56</v>
+      </c>
+      <c r="T21" s="458"/>
+      <c r="U21" s="458"/>
+      <c r="V21" s="479" t="s">
+        <v>57</v>
+      </c>
+      <c r="W21" s="479"/>
+      <c r="X21" s="479"/>
+      <c r="Y21" s="471" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z21" s="472"/>
+      <c r="AA21" s="473"/>
+      <c r="AB21" s="480" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC21" s="480"/>
+      <c r="AD21" s="480"/>
+      <c r="AE21" s="481" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF21" s="482"/>
+      <c r="AG21" s="482"/>
+      <c r="AH21" s="483" t="s">
+        <v>61</v>
+      </c>
+      <c r="AI21" s="483"/>
+      <c r="AJ21" s="484"/>
     </row>
-    <row r="6" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="J6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>17</v>
-      </c>
+    <row r="22" spans="3:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G22" s="217"/>
+      <c r="H22" s="163"/>
+      <c r="I22" s="163"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="429"/>
+      <c r="N22" s="430"/>
+      <c r="O22" s="431"/>
+      <c r="P22" s="455"/>
+      <c r="Q22" s="456"/>
+      <c r="R22" s="457"/>
+      <c r="S22" s="460"/>
+      <c r="T22" s="460"/>
+      <c r="U22" s="460"/>
+      <c r="V22" s="485"/>
+      <c r="W22" s="485"/>
+      <c r="X22" s="485"/>
+      <c r="Y22" s="486"/>
+      <c r="Z22" s="487"/>
+      <c r="AA22" s="488"/>
+      <c r="AB22" s="489"/>
+      <c r="AC22" s="489"/>
+      <c r="AD22" s="489"/>
+      <c r="AE22" s="490"/>
+      <c r="AF22" s="491"/>
+      <c r="AG22" s="491"/>
+      <c r="AH22" s="492"/>
+      <c r="AI22" s="492"/>
+      <c r="AJ22" s="493"/>
     </row>
-    <row r="7" spans="1:33" ht="15" customHeight="1">
-      <c r="A7" s="551" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="125"/>
-      <c r="E7" s="126"/>
-      <c r="F7" s="127"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="345"/>
-      <c r="K7" s="346"/>
-      <c r="L7" s="347"/>
-      <c r="M7" s="354"/>
-      <c r="N7" s="355"/>
-      <c r="O7" s="356"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="77"/>
-      <c r="T7" s="78"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="381"/>
-      <c r="W7" s="382"/>
-      <c r="X7" s="383"/>
-      <c r="Y7" s="164"/>
-      <c r="Z7" s="165"/>
-      <c r="AA7" s="166"/>
-      <c r="AB7" s="254"/>
-      <c r="AC7" s="255"/>
-      <c r="AD7" s="256"/>
-      <c r="AE7" s="257"/>
-      <c r="AF7" s="258"/>
-      <c r="AG7" s="259"/>
-    </row>
-    <row r="8" spans="1:33" ht="15" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="138" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="139"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="200"/>
-      <c r="I8" s="201"/>
-      <c r="J8" s="348" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="349"/>
-      <c r="L8" s="350"/>
-      <c r="M8" s="438" t="s">
-        <v>76</v>
-      </c>
-      <c r="N8" s="439"/>
-      <c r="O8" s="440"/>
-      <c r="P8" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="42"/>
-      <c r="R8" s="43"/>
-      <c r="S8" s="89" t="s">
-        <v>4</v>
-      </c>
-      <c r="T8" s="90"/>
-      <c r="U8" s="91"/>
-      <c r="V8" s="384" t="s">
-        <v>21</v>
-      </c>
-      <c r="W8" s="385"/>
-      <c r="X8" s="386"/>
-      <c r="Y8" s="176" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z8" s="177"/>
-      <c r="AA8" s="178"/>
-      <c r="AB8" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC8" s="114"/>
-      <c r="AD8" s="115"/>
-      <c r="AE8" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="AF8" s="66"/>
-      <c r="AG8" s="67"/>
-    </row>
-    <row r="9" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D9" s="151"/>
-      <c r="E9" s="152"/>
-      <c r="F9" s="153"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="351"/>
-      <c r="K9" s="352"/>
-      <c r="L9" s="353"/>
-      <c r="M9" s="357"/>
-      <c r="N9" s="358"/>
-      <c r="O9" s="359"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="101"/>
-      <c r="T9" s="102"/>
-      <c r="U9" s="103"/>
-      <c r="V9" s="387"/>
-      <c r="W9" s="388"/>
-      <c r="X9" s="389"/>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="189"/>
-      <c r="AA9" s="190"/>
-      <c r="AB9" s="260"/>
-      <c r="AC9" s="261"/>
-      <c r="AD9" s="262"/>
-      <c r="AE9" s="263"/>
-      <c r="AF9" s="264"/>
-      <c r="AG9" s="265"/>
-    </row>
-    <row r="10" spans="1:33" ht="15" customHeight="1" thickBot="1"/>
-    <row r="11" spans="1:33" ht="15" customHeight="1">
-      <c r="D11" s="128"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="130"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="411"/>
-      <c r="K11" s="412"/>
-      <c r="L11" s="413"/>
-      <c r="M11" s="360"/>
-      <c r="N11" s="361"/>
-      <c r="O11" s="362"/>
-      <c r="P11" s="32"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="34"/>
-      <c r="S11" s="80"/>
-      <c r="T11" s="81"/>
-      <c r="U11" s="82"/>
-      <c r="V11" s="396"/>
-      <c r="W11" s="397"/>
-      <c r="X11" s="398"/>
-      <c r="Y11" s="167"/>
-      <c r="Z11" s="168"/>
-      <c r="AA11" s="169"/>
-      <c r="AB11" s="218"/>
-      <c r="AC11" s="219"/>
-      <c r="AD11" s="220"/>
-      <c r="AE11" s="221"/>
-      <c r="AF11" s="222"/>
-      <c r="AG11" s="223"/>
-    </row>
-    <row r="12" spans="1:33" ht="15" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="141" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="142"/>
-      <c r="F12" s="143"/>
-      <c r="G12" s="202" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="203"/>
-      <c r="I12" s="204"/>
-      <c r="J12" s="414" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="415"/>
-      <c r="L12" s="416"/>
-      <c r="M12" s="363" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="364"/>
-      <c r="O12" s="365"/>
-      <c r="P12" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="46"/>
-      <c r="S12" s="92" t="s">
-        <v>12</v>
-      </c>
-      <c r="T12" s="93"/>
-      <c r="U12" s="94"/>
-      <c r="V12" s="399" t="s">
-        <v>24</v>
-      </c>
-      <c r="W12" s="400"/>
-      <c r="X12" s="401"/>
-      <c r="Y12" s="179" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z12" s="180"/>
-      <c r="AA12" s="181"/>
-      <c r="AB12" s="116" t="s">
-        <v>13</v>
-      </c>
-      <c r="AC12" s="117"/>
-      <c r="AD12" s="118"/>
-      <c r="AE12" s="68" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF12" s="69"/>
-      <c r="AG12" s="70"/>
-    </row>
-    <row r="13" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D13" s="154"/>
-      <c r="E13" s="155"/>
-      <c r="F13" s="156"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="417"/>
-      <c r="K13" s="418"/>
-      <c r="L13" s="419"/>
-      <c r="M13" s="366"/>
-      <c r="N13" s="367"/>
-      <c r="O13" s="368"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="57"/>
-      <c r="R13" s="58"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="105"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="402"/>
-      <c r="W13" s="403"/>
-      <c r="X13" s="404"/>
-      <c r="Y13" s="191"/>
-      <c r="Z13" s="192"/>
-      <c r="AA13" s="193"/>
-      <c r="AB13" s="224"/>
-      <c r="AC13" s="225"/>
-      <c r="AD13" s="226"/>
-      <c r="AE13" s="227"/>
-      <c r="AF13" s="228"/>
-      <c r="AG13" s="229"/>
-    </row>
-    <row r="14" spans="1:33" ht="15" customHeight="1">
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="133"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="420"/>
-      <c r="K14" s="421"/>
-      <c r="L14" s="422"/>
-      <c r="M14" s="369"/>
-      <c r="N14" s="370"/>
-      <c r="O14" s="371"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="83"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="390"/>
-      <c r="W14" s="391"/>
-      <c r="X14" s="392"/>
-      <c r="Y14" s="170"/>
-      <c r="Z14" s="171"/>
-      <c r="AA14" s="172"/>
-      <c r="AB14" s="230"/>
-      <c r="AC14" s="231"/>
-      <c r="AD14" s="232"/>
-      <c r="AE14" s="233"/>
-      <c r="AF14" s="234"/>
-      <c r="AG14" s="235"/>
-    </row>
-    <row r="15" spans="1:33" ht="15" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="144" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="145"/>
-      <c r="F15" s="146"/>
-      <c r="G15" s="205" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="206"/>
-      <c r="I15" s="207"/>
-      <c r="J15" s="420" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="421"/>
-      <c r="L15" s="422"/>
-      <c r="M15" s="369" t="s">
-        <v>58</v>
-      </c>
-      <c r="N15" s="370"/>
-      <c r="O15" s="371"/>
-      <c r="P15" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q15" s="48"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="95" t="s">
-        <v>60</v>
-      </c>
-      <c r="T15" s="96"/>
-      <c r="U15" s="97"/>
-      <c r="V15" s="390" t="s">
-        <v>61</v>
-      </c>
-      <c r="W15" s="391"/>
-      <c r="X15" s="392"/>
-      <c r="Y15" s="182" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z15" s="183"/>
-      <c r="AA15" s="184"/>
-      <c r="AB15" s="119" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC15" s="120"/>
-      <c r="AD15" s="121"/>
-      <c r="AE15" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF15" s="72"/>
-      <c r="AG15" s="73"/>
-    </row>
-    <row r="16" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D16" s="157"/>
-      <c r="E16" s="158"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="423"/>
-      <c r="K16" s="424"/>
-      <c r="L16" s="425"/>
-      <c r="M16" s="372"/>
-      <c r="N16" s="373"/>
-      <c r="O16" s="374"/>
-      <c r="P16" s="59"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="61"/>
-      <c r="S16" s="107"/>
-      <c r="T16" s="108"/>
-      <c r="U16" s="109"/>
-      <c r="V16" s="393"/>
-      <c r="W16" s="394"/>
-      <c r="X16" s="395"/>
-      <c r="Y16" s="194"/>
-      <c r="Z16" s="195"/>
-      <c r="AA16" s="196"/>
-      <c r="AB16" s="236"/>
-      <c r="AC16" s="237"/>
-      <c r="AD16" s="238"/>
-      <c r="AE16" s="239"/>
-      <c r="AF16" s="240"/>
-      <c r="AG16" s="241"/>
-    </row>
-    <row r="17" spans="1:33" ht="15" customHeight="1">
-      <c r="D17" s="134"/>
-      <c r="E17" s="135"/>
-      <c r="F17" s="136"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="426"/>
-      <c r="K17" s="427"/>
-      <c r="L17" s="428"/>
-      <c r="M17" s="375"/>
-      <c r="N17" s="376"/>
-      <c r="O17" s="377"/>
-      <c r="P17" s="38"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="86"/>
-      <c r="T17" s="87"/>
-      <c r="U17" s="88"/>
-      <c r="V17" s="405"/>
-      <c r="W17" s="406"/>
-      <c r="X17" s="407"/>
-      <c r="Y17" s="173"/>
-      <c r="Z17" s="174"/>
-      <c r="AA17" s="175"/>
-      <c r="AB17" s="242"/>
-      <c r="AC17" s="243"/>
-      <c r="AD17" s="244"/>
-      <c r="AE17" s="245"/>
-      <c r="AF17" s="246"/>
-      <c r="AG17" s="247"/>
-    </row>
-    <row r="18" spans="1:33" ht="15" customHeight="1">
-      <c r="A18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="147" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="148"/>
-      <c r="F18" s="149"/>
-      <c r="G18" s="208" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="209"/>
-      <c r="I18" s="210"/>
-      <c r="J18" s="426" t="s">
-        <v>18</v>
-      </c>
-      <c r="K18" s="427"/>
-      <c r="L18" s="428"/>
-      <c r="M18" s="375" t="s">
-        <v>67</v>
-      </c>
-      <c r="N18" s="376"/>
-      <c r="O18" s="377"/>
-      <c r="P18" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="52"/>
-      <c r="S18" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="T18" s="99"/>
-      <c r="U18" s="100"/>
-      <c r="V18" s="405" t="s">
-        <v>19</v>
-      </c>
-      <c r="W18" s="406"/>
-      <c r="X18" s="407"/>
-      <c r="Y18" s="185" t="s">
-        <v>68</v>
-      </c>
-      <c r="Z18" s="186"/>
-      <c r="AA18" s="187"/>
-      <c r="AB18" s="122" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC18" s="123"/>
-      <c r="AD18" s="124"/>
-      <c r="AE18" s="74" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF18" s="75"/>
-      <c r="AG18" s="76"/>
-    </row>
-    <row r="19" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D19" s="160"/>
-      <c r="E19" s="161"/>
-      <c r="F19" s="162"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="429"/>
-      <c r="K19" s="430"/>
-      <c r="L19" s="431"/>
-      <c r="M19" s="378"/>
-      <c r="N19" s="379"/>
-      <c r="O19" s="380"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="64"/>
-      <c r="S19" s="110"/>
-      <c r="T19" s="111"/>
-      <c r="U19" s="112"/>
-      <c r="V19" s="408"/>
-      <c r="W19" s="409"/>
-      <c r="X19" s="410"/>
-      <c r="Y19" s="197"/>
-      <c r="Z19" s="198"/>
-      <c r="AA19" s="199"/>
-      <c r="AB19" s="248"/>
-      <c r="AC19" s="249"/>
-      <c r="AD19" s="250"/>
-      <c r="AE19" s="251"/>
-      <c r="AF19" s="252"/>
-      <c r="AG19" s="253"/>
-    </row>
-    <row r="20" spans="1:33" ht="15" customHeight="1">
-      <c r="D20" s="215"/>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="426"/>
-      <c r="K20" s="427"/>
-      <c r="L20" s="428"/>
-      <c r="M20" s="452"/>
-      <c r="N20" s="453"/>
-      <c r="O20" s="454"/>
-      <c r="P20" s="459"/>
-      <c r="Q20" s="459"/>
-      <c r="R20" s="459"/>
-      <c r="S20" s="470"/>
-      <c r="T20" s="470"/>
-      <c r="U20" s="470"/>
-      <c r="V20" s="471"/>
-      <c r="W20" s="472"/>
-      <c r="X20" s="473"/>
-      <c r="Y20" s="474"/>
-      <c r="Z20" s="474"/>
-      <c r="AA20" s="474"/>
-      <c r="AB20" s="475"/>
-      <c r="AC20" s="476"/>
-      <c r="AD20" s="476"/>
-      <c r="AE20" s="477"/>
-      <c r="AF20" s="477"/>
-      <c r="AG20" s="478"/>
-    </row>
-    <row r="21" spans="1:33" ht="15" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="216" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="150"/>
-      <c r="F21" s="150"/>
-      <c r="G21" s="211" t="s">
-        <v>80</v>
-      </c>
-      <c r="H21" s="211"/>
-      <c r="I21" s="211"/>
-      <c r="J21" s="426" t="s">
-        <v>18</v>
-      </c>
-      <c r="K21" s="427"/>
-      <c r="L21" s="428"/>
-      <c r="M21" s="452" t="s">
-        <v>81</v>
-      </c>
-      <c r="N21" s="453"/>
-      <c r="O21" s="454"/>
-      <c r="P21" s="458" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q21" s="458"/>
-      <c r="R21" s="458"/>
-      <c r="S21" s="479" t="s">
-        <v>83</v>
-      </c>
-      <c r="T21" s="479"/>
-      <c r="U21" s="479"/>
-      <c r="V21" s="471" t="s">
-        <v>84</v>
-      </c>
-      <c r="W21" s="472"/>
-      <c r="X21" s="473"/>
-      <c r="Y21" s="480" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z21" s="480"/>
-      <c r="AA21" s="480"/>
-      <c r="AB21" s="481" t="s">
-        <v>86</v>
-      </c>
-      <c r="AC21" s="482"/>
-      <c r="AD21" s="482"/>
-      <c r="AE21" s="483" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF21" s="483"/>
-      <c r="AG21" s="484"/>
-    </row>
-    <row r="22" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D22" s="217"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="163"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="429"/>
-      <c r="K22" s="430"/>
-      <c r="L22" s="431"/>
-      <c r="M22" s="455"/>
-      <c r="N22" s="456"/>
-      <c r="O22" s="457"/>
-      <c r="P22" s="460"/>
-      <c r="Q22" s="460"/>
-      <c r="R22" s="460"/>
-      <c r="S22" s="485"/>
-      <c r="T22" s="485"/>
-      <c r="U22" s="485"/>
-      <c r="V22" s="486"/>
-      <c r="W22" s="487"/>
-      <c r="X22" s="488"/>
-      <c r="Y22" s="489"/>
-      <c r="Z22" s="489"/>
-      <c r="AA22" s="489"/>
-      <c r="AB22" s="490"/>
-      <c r="AC22" s="491"/>
-      <c r="AD22" s="491"/>
-      <c r="AE22" s="492"/>
-      <c r="AF22" s="492"/>
-      <c r="AG22" s="493"/>
-    </row>
-    <row r="23" spans="1:33" ht="15" customHeight="1">
-      <c r="D23" s="536"/>
-      <c r="E23" s="537"/>
-      <c r="F23" s="538"/>
-      <c r="G23" s="539"/>
-      <c r="H23" s="540"/>
-      <c r="I23" s="541"/>
-      <c r="J23" s="432"/>
-      <c r="K23" s="433"/>
-      <c r="L23" s="434"/>
+    <row r="23" spans="3:36" ht="15" customHeight="1">
+      <c r="G23" s="536"/>
+      <c r="H23" s="537"/>
+      <c r="I23" s="538"/>
+      <c r="J23" s="539"/>
+      <c r="K23" s="540"/>
+      <c r="L23" s="541"/>
       <c r="M23" s="432"/>
       <c r="N23" s="433"/>
       <c r="O23" s="434"/>
-      <c r="P23" s="461"/>
-      <c r="Q23" s="462"/>
-      <c r="R23" s="463"/>
-      <c r="S23" s="494"/>
-      <c r="T23" s="495"/>
-      <c r="U23" s="496"/>
-      <c r="V23" s="497"/>
-      <c r="W23" s="498"/>
-      <c r="X23" s="499"/>
-      <c r="Y23" s="500"/>
-      <c r="Z23" s="501"/>
-      <c r="AA23" s="502"/>
-      <c r="AB23" s="503"/>
-      <c r="AC23" s="504"/>
-      <c r="AD23" s="505"/>
-      <c r="AE23" s="506"/>
-      <c r="AF23" s="507"/>
-      <c r="AG23" s="508"/>
+      <c r="P23" s="432"/>
+      <c r="Q23" s="433"/>
+      <c r="R23" s="434"/>
+      <c r="S23" s="461"/>
+      <c r="T23" s="462"/>
+      <c r="U23" s="463"/>
+      <c r="V23" s="494"/>
+      <c r="W23" s="495"/>
+      <c r="X23" s="496"/>
+      <c r="Y23" s="497"/>
+      <c r="Z23" s="498"/>
+      <c r="AA23" s="499"/>
+      <c r="AB23" s="500"/>
+      <c r="AC23" s="501"/>
+      <c r="AD23" s="502"/>
+      <c r="AE23" s="503"/>
+      <c r="AF23" s="504"/>
+      <c r="AG23" s="505"/>
+      <c r="AH23" s="506"/>
+      <c r="AI23" s="507"/>
+      <c r="AJ23" s="508"/>
     </row>
-    <row r="24" spans="1:33" ht="15" customHeight="1">
-      <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="542" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="543"/>
-      <c r="F24" s="544"/>
-      <c r="G24" s="212" t="s">
-        <v>88</v>
-      </c>
-      <c r="H24" s="213"/>
-      <c r="I24" s="214"/>
-      <c r="J24" s="432" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" s="433"/>
-      <c r="L24" s="434"/>
+    <row r="24" spans="3:36" ht="15" customHeight="1">
+      <c r="D24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="542" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="543"/>
+      <c r="I24" s="544"/>
+      <c r="J24" s="212" t="s">
+        <v>62</v>
+      </c>
+      <c r="K24" s="213"/>
+      <c r="L24" s="214"/>
       <c r="M24" s="432" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="N24" s="433"/>
       <c r="O24" s="434"/>
-      <c r="P24" s="464" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q24" s="465"/>
-      <c r="R24" s="466"/>
-      <c r="S24" s="509" t="s">
-        <v>91</v>
-      </c>
-      <c r="T24" s="510"/>
-      <c r="U24" s="511"/>
-      <c r="V24" s="497" t="s">
-        <v>92</v>
-      </c>
-      <c r="W24" s="498"/>
-      <c r="X24" s="499"/>
-      <c r="Y24" s="512" t="s">
-        <v>93</v>
-      </c>
-      <c r="Z24" s="513"/>
-      <c r="AA24" s="514"/>
-      <c r="AB24" s="515" t="s">
-        <v>94</v>
-      </c>
-      <c r="AC24" s="516"/>
-      <c r="AD24" s="517"/>
-      <c r="AE24" s="518" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF24" s="519"/>
-      <c r="AG24" s="520"/>
+      <c r="P24" s="432" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q24" s="433"/>
+      <c r="R24" s="434"/>
+      <c r="S24" s="464" t="s">
+        <v>64</v>
+      </c>
+      <c r="T24" s="465"/>
+      <c r="U24" s="466"/>
+      <c r="V24" s="509" t="s">
+        <v>65</v>
+      </c>
+      <c r="W24" s="510"/>
+      <c r="X24" s="511"/>
+      <c r="Y24" s="497" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z24" s="498"/>
+      <c r="AA24" s="499"/>
+      <c r="AB24" s="512" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC24" s="513"/>
+      <c r="AD24" s="514"/>
+      <c r="AE24" s="515" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF24" s="516"/>
+      <c r="AG24" s="517"/>
+      <c r="AH24" s="518" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI24" s="519"/>
+      <c r="AJ24" s="520"/>
     </row>
-    <row r="25" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="D25" s="545"/>
-      <c r="E25" s="546"/>
-      <c r="F25" s="547"/>
-      <c r="G25" s="548"/>
-      <c r="H25" s="549"/>
-      <c r="I25" s="550"/>
-      <c r="J25" s="435"/>
-      <c r="K25" s="436"/>
-      <c r="L25" s="437"/>
+    <row r="25" spans="3:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G25" s="545"/>
+      <c r="H25" s="546"/>
+      <c r="I25" s="547"/>
+      <c r="J25" s="548"/>
+      <c r="K25" s="549"/>
+      <c r="L25" s="550"/>
       <c r="M25" s="435"/>
       <c r="N25" s="436"/>
       <c r="O25" s="437"/>
-      <c r="P25" s="467"/>
-      <c r="Q25" s="468"/>
-      <c r="R25" s="469"/>
-      <c r="S25" s="521"/>
-      <c r="T25" s="522"/>
-      <c r="U25" s="523"/>
-      <c r="V25" s="524"/>
-      <c r="W25" s="525"/>
-      <c r="X25" s="526"/>
-      <c r="Y25" s="527"/>
-      <c r="Z25" s="528"/>
-      <c r="AA25" s="529"/>
-      <c r="AB25" s="530"/>
-      <c r="AC25" s="531"/>
-      <c r="AD25" s="532"/>
-      <c r="AE25" s="533"/>
-      <c r="AF25" s="534"/>
-      <c r="AG25" s="535"/>
+      <c r="P25" s="435"/>
+      <c r="Q25" s="436"/>
+      <c r="R25" s="437"/>
+      <c r="S25" s="467"/>
+      <c r="T25" s="468"/>
+      <c r="U25" s="469"/>
+      <c r="V25" s="521"/>
+      <c r="W25" s="522"/>
+      <c r="X25" s="523"/>
+      <c r="Y25" s="524"/>
+      <c r="Z25" s="525"/>
+      <c r="AA25" s="526"/>
+      <c r="AB25" s="527"/>
+      <c r="AC25" s="528"/>
+      <c r="AD25" s="529"/>
+      <c r="AE25" s="530"/>
+      <c r="AF25" s="531"/>
+      <c r="AG25" s="532"/>
+      <c r="AH25" s="533"/>
+      <c r="AI25" s="534"/>
+      <c r="AJ25" s="535"/>
     </row>
-    <row r="27" spans="1:33" ht="15" customHeight="1">
-      <c r="D27" s="551" t="s">
-        <v>71</v>
+    <row r="27" spans="3:36" ht="15" customHeight="1">
+      <c r="G27" s="551" t="s">
+        <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:33" ht="15" customHeight="1">
-      <c r="D28" s="1" t="s">
-        <v>45</v>
-      </c>
+    <row r="28" spans="3:36" ht="15" customHeight="1">
       <c r="G28" s="1" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="M28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="3:36" ht="15" customHeight="1" thickBot="1">
+      <c r="S29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="30" spans="3:36" ht="15" customHeight="1">
+      <c r="D30" s="551" t="s">
         <v>47</v>
       </c>
-      <c r="P28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="S28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="V28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y28" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB28" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE28" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="G30" s="266"/>
+      <c r="H30" s="267"/>
+      <c r="I30" s="268"/>
+      <c r="J30" s="274"/>
+      <c r="K30" s="275"/>
+      <c r="L30" s="276"/>
+      <c r="M30" s="282"/>
+      <c r="N30" s="283"/>
+      <c r="O30" s="284"/>
+      <c r="P30" s="291"/>
+      <c r="Q30" s="292"/>
+      <c r="R30" s="293"/>
+      <c r="S30" s="300"/>
+      <c r="T30" s="301"/>
+      <c r="U30" s="302"/>
+      <c r="V30" s="309"/>
+      <c r="W30" s="310"/>
+      <c r="X30" s="311"/>
+      <c r="Y30" s="318"/>
+      <c r="Z30" s="319"/>
+      <c r="AA30" s="320"/>
+      <c r="AB30" s="327"/>
+      <c r="AC30" s="328"/>
+      <c r="AD30" s="329"/>
+      <c r="AE30" s="333"/>
+      <c r="AF30" s="334"/>
+      <c r="AG30" s="335"/>
+      <c r="AH30" s="339"/>
+      <c r="AI30" s="340"/>
+      <c r="AJ30" s="341"/>
     </row>
-    <row r="29" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="P29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V29" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="31" spans="3:36" ht="15" customHeight="1">
+      <c r="C31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" s="441" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="269"/>
+      <c r="I31" s="270"/>
+      <c r="J31" s="442" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="277"/>
+      <c r="L31" s="278"/>
+      <c r="M31" s="285" t="s">
+        <v>5</v>
+      </c>
+      <c r="N31" s="286"/>
+      <c r="O31" s="287"/>
+      <c r="P31" s="294" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q31" s="295"/>
+      <c r="R31" s="296"/>
+      <c r="S31" s="303" t="s">
+        <v>24</v>
+      </c>
+      <c r="T31" s="304"/>
+      <c r="U31" s="305"/>
+      <c r="V31" s="312" t="s">
+        <v>25</v>
+      </c>
+      <c r="W31" s="313"/>
+      <c r="X31" s="314"/>
+      <c r="Y31" s="321" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z31" s="322"/>
+      <c r="AA31" s="323"/>
+      <c r="AB31" s="443" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC31" s="444"/>
+      <c r="AD31" s="445"/>
+      <c r="AE31" s="446" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF31" s="447"/>
+      <c r="AG31" s="448"/>
+      <c r="AH31" s="449" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI31" s="450"/>
+      <c r="AJ31" s="451"/>
     </row>
-    <row r="30" spans="1:33" ht="15" customHeight="1">
-      <c r="A30" s="551" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="266"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="268"/>
-      <c r="G30" s="274"/>
-      <c r="H30" s="275"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="282"/>
-      <c r="K30" s="283"/>
-      <c r="L30" s="284"/>
-      <c r="M30" s="291"/>
-      <c r="N30" s="292"/>
-      <c r="O30" s="293"/>
-      <c r="P30" s="300"/>
-      <c r="Q30" s="301"/>
-      <c r="R30" s="302"/>
-      <c r="S30" s="309"/>
-      <c r="T30" s="310"/>
-      <c r="U30" s="311"/>
-      <c r="V30" s="318"/>
-      <c r="W30" s="319"/>
-      <c r="X30" s="320"/>
-      <c r="Y30" s="327"/>
-      <c r="Z30" s="328"/>
-      <c r="AA30" s="329"/>
-      <c r="AB30" s="333"/>
-      <c r="AC30" s="334"/>
-      <c r="AD30" s="335"/>
-      <c r="AE30" s="339"/>
-      <c r="AF30" s="340"/>
-      <c r="AG30" s="341"/>
-    </row>
-    <row r="31" spans="1:33" ht="15" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="441" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="269"/>
-      <c r="F31" s="270"/>
-      <c r="G31" s="442" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="277"/>
-      <c r="I31" s="278"/>
-      <c r="J31" s="285" t="s">
-        <v>7</v>
-      </c>
-      <c r="K31" s="286"/>
-      <c r="L31" s="287"/>
-      <c r="M31" s="294" t="s">
-        <v>27</v>
-      </c>
-      <c r="N31" s="295"/>
-      <c r="O31" s="296"/>
-      <c r="P31" s="303" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q31" s="304"/>
-      <c r="R31" s="305"/>
-      <c r="S31" s="312" t="s">
-        <v>29</v>
-      </c>
-      <c r="T31" s="313"/>
-      <c r="U31" s="314"/>
-      <c r="V31" s="321" t="s">
-        <v>30</v>
-      </c>
-      <c r="W31" s="322"/>
-      <c r="X31" s="323"/>
-      <c r="Y31" s="443" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z31" s="444"/>
-      <c r="AA31" s="445"/>
-      <c r="AB31" s="446" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC31" s="447"/>
-      <c r="AD31" s="448"/>
-      <c r="AE31" s="449" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF31" s="450"/>
-      <c r="AG31" s="451"/>
-    </row>
-    <row r="32" spans="1:33" ht="15" customHeight="1" thickBot="1">
-      <c r="A32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="271"/>
-      <c r="E32" s="272"/>
-      <c r="F32" s="273"/>
-      <c r="G32" s="279"/>
-      <c r="H32" s="280"/>
-      <c r="I32" s="281"/>
-      <c r="J32" s="288"/>
-      <c r="K32" s="289"/>
-      <c r="L32" s="290"/>
-      <c r="M32" s="297"/>
-      <c r="N32" s="298"/>
-      <c r="O32" s="299"/>
-      <c r="P32" s="306"/>
-      <c r="Q32" s="307"/>
-      <c r="R32" s="308"/>
-      <c r="S32" s="315"/>
-      <c r="T32" s="316"/>
-      <c r="U32" s="317"/>
-      <c r="V32" s="324"/>
-      <c r="W32" s="325"/>
-      <c r="X32" s="326"/>
-      <c r="Y32" s="330"/>
-      <c r="Z32" s="331"/>
-      <c r="AA32" s="332"/>
-      <c r="AB32" s="336"/>
-      <c r="AC32" s="337"/>
-      <c r="AD32" s="338"/>
-      <c r="AE32" s="342"/>
-      <c r="AF32" s="343"/>
-      <c r="AG32" s="344"/>
+    <row r="32" spans="3:36" ht="15" customHeight="1" thickBot="1">
+      <c r="G32" s="271"/>
+      <c r="H32" s="272"/>
+      <c r="I32" s="273"/>
+      <c r="J32" s="279"/>
+      <c r="K32" s="280"/>
+      <c r="L32" s="281"/>
+      <c r="M32" s="288"/>
+      <c r="N32" s="289"/>
+      <c r="O32" s="290"/>
+      <c r="P32" s="297"/>
+      <c r="Q32" s="298"/>
+      <c r="R32" s="299"/>
+      <c r="S32" s="306"/>
+      <c r="T32" s="307"/>
+      <c r="U32" s="308"/>
+      <c r="V32" s="315"/>
+      <c r="W32" s="316"/>
+      <c r="X32" s="317"/>
+      <c r="Y32" s="324"/>
+      <c r="Z32" s="325"/>
+      <c r="AA32" s="326"/>
+      <c r="AB32" s="330"/>
+      <c r="AC32" s="331"/>
+      <c r="AD32" s="332"/>
+      <c r="AE32" s="336"/>
+      <c r="AF32" s="337"/>
+      <c r="AG32" s="338"/>
+      <c r="AH32" s="342"/>
+      <c r="AI32" s="343"/>
+      <c r="AJ32" s="344"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>